<commit_message>
excel parsing logic updated
</commit_message>
<xml_diff>
--- a/server/itemlist.xlsx
+++ b/server/itemlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raghav Raj Sobti\Desktop\fresh\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B26EF972-49B7-45F7-BE66-3EAE39F7A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A92BDD2-8E71-4A6A-8530-119304C8A07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
     <t>705678492</t>
   </si>
   <si>
-    <t>Testing first item</t>
+    <t>Testing Excel item</t>
   </si>
 </sst>
 </file>
@@ -993,12 +993,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>196</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>96</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>97</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>98</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>98</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>99</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>101</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>101</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>102</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>102</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>103</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>103</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>107</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>108</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>108</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>109</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>109</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>111</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>111</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>112</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>112</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>113</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>113</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>114</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>115</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>116</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>116</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>118</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>118</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>118</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>118</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>120</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>120</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>122</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>122</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>125</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>125</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>126</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>126</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>128</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>128</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>129</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>129</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>130</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>130</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>131</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>131</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>132</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>132</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>133</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>133</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>134</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>135</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>135</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>136</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>136</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>138</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>138</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>140</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>140</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>141</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>141</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>142</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>142</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>143</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>143</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>144</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>144</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>146</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>150</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>150</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>152</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>152</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>153</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>153</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>154</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>154</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>155</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>155</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>156</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>156</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>157</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>157</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>158</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>158</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>159</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>159</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>161</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>161</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>162</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>162</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>164</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>164</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>166</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>169</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>169</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>171</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>173</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>173</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>174</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>174</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>175</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>175</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>177</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>177</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>178</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>178</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>179</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>179</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>181</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>181</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>183</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>183</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>184</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>184</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>185</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>185</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>186</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>186</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>188</v>
       </c>
@@ -7555,7 +7555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>188</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>189</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>189</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>190</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>190</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>191</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>193</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>194</v>
       </c>

</xml_diff>